<commit_message>
Here is a nice run
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -415,7 +415,7 @@
         <v>37</v>
       </c>
       <c r="F2">
-        <v>0.05921016699999999</v>
+        <v>0.058962667</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -435,7 +435,7 @@
         <v>414</v>
       </c>
       <c r="F3">
-        <v>5.972509415999999</v>
+        <v>5.968093167</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -455,7 +455,7 @@
         <v>1466</v>
       </c>
       <c r="F4">
-        <v>61.73076775000001</v>
+        <v>61.12055950000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UCS heuristic 1 done, will refactor later
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Puzzle Number</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>No solution.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,53 +406,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>37</v>
       </c>
       <c r="F2">
-        <v>0.05805004100000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>414</v>
-      </c>
-      <c r="F3">
-        <v>5.944643834000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>1466</v>
-      </c>
-      <c r="F4">
-        <v>60.83730875</v>
+        <v>0.057912333</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed gn and problem for others
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Puzzle Number</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>No solution.</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -409,53 +406,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E2">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F2">
-        <v>0.05805004100000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>414</v>
-      </c>
-      <c r="F3">
-        <v>5.944643834000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>1466</v>
-      </c>
-      <c r="F4">
-        <v>60.83730875</v>
+        <v>152.9034914</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Heuristics calculating what it needs to
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -406,13 +406,13 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="E2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>152.9034914</v>
+        <v>0.04305529999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>